<commit_message>
datasoftware srl - intellilab - 3
corretto case test id 446
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DATASOFTWARE/DATASOFTWARE_SRL/INTELLILAB/3/report-checklist.xlsx
+++ b/GATEWAY/A1#111DATASOFTWARE/DATASOFTWARE_SRL/INTELLILAB/3/report-checklist.xlsx
@@ -780,13 +780,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-07-10T11:09:42.8829628+02:00</t>
-  </si>
-  <si>
-    <t>4022662c3e5cb238</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.d7eefc7b8a503d0a01e7fee30565a19e23bb25a16cb91c59b98a1691ee0cebae.64e7acb3b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-08-05T16:00:02.5612529+02:00</t>
+  </si>
+  <si>
+    <t>2a5f5a35af310796</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.d7eefc7b8a503d0a01e7fee30565a19e23bb25a16cb91c59b98a1691ee0cebae.05fffd6c2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -1161,15 +1161,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -2500,12 +2500,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{78881865-1A76-4B43-9EB1-8976FA7D4E65}">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{B8A871DD-197E-4F09-8B6F-B560CC86408C}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{CD222A37-AA01-41B8-9395-7E2058BFD7AC}">
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{824D28E0-1494-422C-9A8F-89136AA38A6A}">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
@@ -3894,7 +3894,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4571428571429" defaultRowHeight="15" customHeight="1"/>
@@ -6089,7 +6089,7 @@
         <v>166</v>
       </c>
       <c r="F54" s="28">
-        <v>45483</v>
+        <v>45509</v>
       </c>
       <c r="G54" s="29" t="s">
         <v>167</v>
@@ -10574,7 +10574,7 @@
       <c r="W630" s="47"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:W55">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A9:W55" etc:filterBottomFollowUsedRange="0">
     <sortState ref="A9:W55">
       <sortCondition ref="A9"/>
     </sortState>
@@ -10590,13 +10590,13 @@
     <mergeCell ref="A3:B5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J15;M15:N15;P15:R15;J16;M16:N16;P16:R16;J17;M17:N17;P17:R17;J18;M18:N18;P18:R18;J19;M19:N19;P19:R19;J20;M20:N20;P20:R20;J53;M53:N53;P53:R53;J10:J14;J21:J31;J32:J50;J51:J52;J54:J55;M10:N14;P10:R14;P21:R31;P32:R50;P51:R52;P54:R55;M21:N31;M32:N50;M51:N52;M54:N55">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J55;M10:N55;P10:R55">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K15;K16;K17;K18;K19;K20;K53;K10:K14;K21:K31;K32:K50;K51:K52;K54:K55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K55">
       <formula1>'LISTA VALORI'!$A$2:$A$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T15;T16;T17;T18;T19;T20;T53;T10:T14;T21:T31;T32:T50;T51:T52;T54:T55">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T10:T55">
       <formula1>Sheet1!$A$2:$A$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -11796,7 +11796,7 @@
     <row r="959" ht="15.75" customHeight="1"/>
     <row r="960" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:G11">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G11" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
update documents - id 446
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DATASOFTWARE/DATASOFTWARE_SRL/INTELLILAB/3/report-checklist.xlsx
+++ b/GATEWAY/A1#111DATASOFTWARE/DATASOFTWARE_SRL/INTELLILAB/3/report-checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13980" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -780,13 +780,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-08-05T16:00:02.5612529+02:00</t>
-  </si>
-  <si>
-    <t>2a5f5a35af310796</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.d7eefc7b8a503d0a01e7fee30565a19e23bb25a16cb91c59b98a1691ee0cebae.05fffd6c2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-08-06T18:20:59.117547+02:00</t>
+  </si>
+  <si>
+    <t>8618e763049b13f2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.d7eefc7b8a503d0a01e7fee30565a19e23bb25a16cb91c59b98a1691ee0cebae.bf0e673968^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -1161,15 +1161,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -2500,12 +2500,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{B8A871DD-197E-4F09-8B6F-B560CC86408C}">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{134AF131-5099-4D55-A38E-114FBEC90476}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{824D28E0-1494-422C-9A8F-89136AA38A6A}">
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{D988CE77-E441-4498-BDC6-921D14945C58}">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
@@ -3894,7 +3894,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4571428571429" defaultRowHeight="15" customHeight="1"/>
@@ -6089,7 +6089,7 @@
         <v>166</v>
       </c>
       <c r="F54" s="28">
-        <v>45509</v>
+        <v>45510</v>
       </c>
       <c r="G54" s="29" t="s">
         <v>167</v>

</xml_diff>